<commit_message>
Add and Withdraw Page Updated
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N57"/>
+  <dimension ref="A1:O40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,25 +469,30 @@
       </c>
       <c r="J1" t="inlineStr">
         <is>
+          <t>Row</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
           <t>Box</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>Plant Name</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>Part No</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>Tag</t>
         </is>
@@ -501,37 +506,37 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>CONTROL VALVE</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>8</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>2''</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>CV</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>150</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>STORE 1</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -541,27 +546,32 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2223232323</t>
+          <t>1</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>MASONEILAN CONTROL VALVE</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>REFORMER 2</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>REF02-CV-150</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>--</t>
         </is>
       </c>
     </row>
@@ -578,7 +588,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -588,7 +598,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>pt</t>
+          <t>PT</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -603,37 +613,42 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>YOKOGAWA PRESSURE TRANSMITTER</t>
+          <t>2</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
+          <t>PRESSURE</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
           <t>REFORMER 2</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
+      <c r="N3" t="inlineStr">
         <is>
           <t>REF02-PT-150</t>
         </is>
       </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>PT-6001</t>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>--</t>
         </is>
       </c>
     </row>
@@ -650,27 +665,27 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>2''</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>CONTROL VALVE</t>
+          <t>CV</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>150</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>STORE 1</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -685,27 +700,33 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>50</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>CONTROL VALVE - MASONEILAN</t>
+          <t>1</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
+          <t>MASONEILAN CONTROL VALVE
+Item no 23</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
           <t>REFORMER 2</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>REF02-CV-2</t>
-        </is>
-      </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>TV-6001</t>
+          <t>REF02-CV-150</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>--</t>
         </is>
       </c>
     </row>
@@ -717,12 +738,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>PRESSURE</t>
+          <t>SOLENOID VALVE</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -732,12 +753,12 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>PT</t>
+          <t>SV</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>24VDC</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -747,37 +768,42 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>1111</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>444</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>YOKOGAWA</t>
+          <t>1</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
+          <t>SOLENOID VALVE SPARE FROM REF02</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
           <t>REFORMER 2</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>REF02-PT-100</t>
-        </is>
-      </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>PT-6002</t>
+          <t>REF02-SV-24VDC</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>--</t>
         </is>
       </c>
     </row>
@@ -789,27 +815,27 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>PRESSURE</t>
+          <t>POWER SUPPLY</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>0</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.6</t>
+          <t>--</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>PT</t>
+          <t>PSU</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>24V 10A</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -824,32 +850,37 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>YOKOGAWA</t>
+          <t>5</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>REFORMER 2</t>
+          <t>POWER SUPPLY</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>REF02-PT-101</t>
+          <t>CHEMEX</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>PT-6003</t>
+          <t>CHE-PSU-24V 10A</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>SOLA</t>
         </is>
       </c>
     </row>
@@ -861,27 +892,27 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>PRESSURE</t>
+          <t>SHUTOFF VALVE</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>21</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.7</t>
+          <t>0.5</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>PT</t>
+          <t>XV</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>150</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -896,32 +927,37 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>22</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>YOKOGAWA</t>
+          <t>1</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>REFORMER 2</t>
+          <t>SHUTOFF VALVE</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>REF02-PT-102</t>
+          <t>FLARE</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>PT-6004</t>
+          <t>FLA-XV-150</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>--</t>
         </is>
       </c>
     </row>
@@ -933,27 +969,27 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>PRESSURE</t>
+          <t>FLAME SENSOR</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0.8</t>
+          <t>--</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>PT</t>
+          <t>FLAME SENSOR</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>24VDC</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -968,32 +1004,37 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>YOKOGAWA</t>
+          <t>1</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
+          <t>FLAME SENSOR . NO NC TYPE . ANALOG OUTPUT TYPE</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
           <t>REFORMER 2</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>REF02-PT-103</t>
-        </is>
-      </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>PT-6005</t>
+          <t>REF02-FLAME SENSOR-24VDC</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>--</t>
         </is>
       </c>
     </row>
@@ -1005,22 +1046,22 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>PRESSURE</t>
+          <t>BALL VALVE</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>0</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0.9</t>
+          <t>0.5''</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>PT</t>
+          <t>MECHANICAL</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1040,32 +1081,37 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>YOKOGAWA</t>
+          <t>1</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>REFORMER 2</t>
+          <t>BALL VALVE</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>REF02-PT-104</t>
+          <t>SPARE</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>PT-6006</t>
+          <t>SPA-MECHANICAL-100</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>--</t>
         </is>
       </c>
     </row>
@@ -1077,27 +1123,27 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>PRESSURE</t>
+          <t>DI CARD</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0.10</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>PT</t>
+          <t>IO CARD</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -1112,32 +1158,37 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>YOKOGAWA</t>
+          <t>PLC</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
+          <t>AB DI CARD</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
           <t>REFORMER 2</t>
         </is>
       </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>REF02-PT-105</t>
-        </is>
-      </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>PT-6007</t>
+          <t>REF02-IO CARD--</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>5069-IB16</t>
         </is>
       </c>
     </row>
@@ -1149,27 +1200,27 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>PRESSURE</t>
+          <t>Temperature</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>18</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.11</t>
+          <t>0.6</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>PT</t>
+          <t>TT</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>600F</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -1179,37 +1230,42 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>25</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>YOKOGAWA</t>
+          <t>1</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>CHEMAX</t>
+          <t>Temperature Transmitter</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>REF02-PT-106</t>
+          <t>REFORMER 2</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>PT-6008</t>
+          <t>REF02-TT-600F</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>TT-6022</t>
         </is>
       </c>
     </row>
@@ -1221,67 +1277,58 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
+          <t>PRESSURE TRANSMITTER</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>150</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H12" t="n">
+        <v>2</v>
+      </c>
+      <c r="I12" t="n">
+        <v>4</v>
+      </c>
+      <c r="J12" t="n">
+        <v>3</v>
+      </c>
+      <c r="K12" t="n">
+        <v>2</v>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
           <t>PRESSURE</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>0.12</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>PT</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>YOKOGAWA</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>CHEMAX</t>
-        </is>
-      </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>REF02-PT-107</t>
+          <t>REFORMER 2</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>PT-6009</t>
+          <t>REF02-PT-151</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>--</t>
         </is>
       </c>
     </row>
@@ -1293,32 +1340,32 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>PRESSURE</t>
+          <t>CONTROL VALVE</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>18</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>0.13</t>
+          <t>2''</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>PT</t>
+          <t>CV</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>151</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>STORE 2</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -1328,32 +1375,37 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>YOKOGAWA</t>
+          <t>1</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>ZEHUA</t>
+          <t>MASONEILAN CONTROL VALVE</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>REF02-PT-108</t>
+          <t>REFORMER 2</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>PT-6010</t>
+          <t>REF02-CV-151</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>--</t>
         </is>
       </c>
     </row>
@@ -1365,27 +1417,27 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>PRESSURE</t>
+          <t>SOLENOID VALVE</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>20</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>0.14</t>
+          <t>0.6</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>PT</t>
+          <t>SV</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>24VDC</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -1400,32 +1452,37 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>YOKOGAWA</t>
+          <t>1</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>ZEHUA</t>
+          <t>SOLENOID VALVE SPARE FROM REF03</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>REF02-PT-109</t>
+          <t>REFORMER 2</t>
         </is>
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>PT-6011</t>
+          <t>REF02-SV-24VDC</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>--</t>
         </is>
       </c>
     </row>
@@ -1437,27 +1494,27 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>PRESSURE</t>
+          <t>POWER SUPPLY</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>0.15</t>
+          <t>--</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>PT</t>
+          <t>PSU</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>24V 10A</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -1472,32 +1529,37 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>YOKOGAWA</t>
+          <t>5</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>FLARE</t>
+          <t>POWER SUPPLY</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>REF02-PT-110</t>
+          <t>CHEMEX</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>PT-6012</t>
+          <t>CHE-PSU-24V 10A</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>SOLA</t>
         </is>
       </c>
     </row>
@@ -1509,27 +1571,27 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>PRESSURE</t>
+          <t>SHUTOFF VALVE</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>25</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>0.16</t>
+          <t>0.6</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>PT</t>
+          <t>XV</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>150</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -1544,32 +1606,37 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>22</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>YOKOGAWA</t>
+          <t>1</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
+          <t>SHUTOFF VALVE</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
           <t>FLARE</t>
         </is>
       </c>
-      <c r="M16" t="inlineStr">
-        <is>
-          <t>REF02-PT-111</t>
-        </is>
-      </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>PT-6013</t>
+          <t>FLA-XV-151</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>--</t>
         </is>
       </c>
     </row>
@@ -1581,27 +1648,27 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>PRESSURE</t>
+          <t>FLAME SENSOR</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.17</t>
+          <t>--</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>PT</t>
+          <t>FLAME SENSOR</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>24VDC</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -1616,32 +1683,37 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>YOKOGAWA</t>
+          <t>1</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
+          <t>FLAME SENSOR . NO NC TYPE . ANALOG OUTPUT TYPE</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
           <t>REFORMER 2</t>
         </is>
       </c>
-      <c r="M17" t="inlineStr">
-        <is>
-          <t>REF02-PT-112</t>
-        </is>
-      </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>PT-6014</t>
+          <t>REF02-FLAME SENSOR-24VDC</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>--</t>
         </is>
       </c>
     </row>
@@ -1653,22 +1725,22 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>PRESSURE</t>
+          <t>BALL VALVE</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>0</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>0.25</t>
+          <t>0.5''</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>PT</t>
+          <t>MECHANICAL</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1688,32 +1760,37 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>YOKOGAWA</t>
+          <t>1</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>BTX</t>
+          <t>BALL VALVE</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>REF02-PT-120</t>
+          <t>SPARE</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>PT-6022</t>
+          <t>SPA-MECHANICAL-101</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>--</t>
         </is>
       </c>
     </row>
@@ -1725,27 +1802,27 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>PRESSURE</t>
+          <t>DI CARD</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>0.26</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>PT</t>
+          <t>IO CARD AB</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -1760,32 +1837,37 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>YOKOGAWA</t>
+          <t>PLC-02</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>BTX</t>
+          <t>AB DI CARD</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>REF02-PT-121</t>
+          <t>REFORMER 2</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>PT-6023</t>
+          <t>REF02-IO CARD AB--</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>5069-IB17</t>
         </is>
       </c>
     </row>
@@ -1797,27 +1879,27 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>PRESSURE</t>
+          <t>Temperature</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>20</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>0.27</t>
+          <t>0.7</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>PT</t>
+          <t>TT</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>600F</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -1827,37 +1909,42 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>YOKOGAWA</t>
+          <t>1</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>BTX</t>
+          <t>Temperature Transmitter</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>REF02-PT-122</t>
+          <t>REFORMER 2</t>
         </is>
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>PT-6024</t>
+          <t>REF02-TT-600F</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>TT-6023</t>
         </is>
       </c>
     </row>
@@ -1869,67 +1956,56 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
+          <t>PRESSURE TRANSMITTER</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>22</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
+      <c r="F21" t="n">
+        <v>150</v>
+      </c>
+      <c r="G21" t="n">
+        <v>1</v>
+      </c>
+      <c r="H21" t="n">
+        <v>2</v>
+      </c>
+      <c r="I21" t="n">
+        <v>4</v>
+      </c>
+      <c r="J21" t="n">
+        <v>3</v>
+      </c>
+      <c r="K21" t="n">
+        <v>2</v>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
           <t>PRESSURE</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>0.28</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>PT</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="J21" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K21" t="inlineStr">
-        <is>
-          <t>YOKOGAWA</t>
-        </is>
-      </c>
-      <c r="L21" t="inlineStr">
-        <is>
-          <t>BTX</t>
-        </is>
-      </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>REF02-PT-123</t>
+          <t>REFORMER 2</t>
         </is>
       </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t>PT-6025</t>
+          <t>REF02-PT-152</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>--</t>
         </is>
       </c>
     </row>
@@ -1941,32 +2017,32 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>PRESSURE</t>
+          <t>CONTROL VALVE</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>18</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>0.29</t>
+          <t>2''</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>PT</t>
+          <t>CV</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>152</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>STORE 3</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
@@ -1976,32 +2052,37 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>555</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>YOKOGAWA</t>
+          <t>1</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>LCP</t>
+          <t>MASONEILAN CONTROL VALVE</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>REF02-PT-124</t>
+          <t>REFORMER 2</t>
         </is>
       </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t>PT-6026</t>
+          <t>REF02-CV-152</t>
+        </is>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>--</t>
         </is>
       </c>
     </row>
@@ -2013,27 +2094,27 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>PRESSURE</t>
+          <t>SOLENOID VALVE</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>30</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0.30</t>
+          <t>0.7</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>PT</t>
+          <t>SV</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>24VDC</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -2048,32 +2129,37 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>YOKOGAWA</t>
+          <t>1</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>LCP</t>
+          <t>SOLENOID VALVE SPARE FROM REF04</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>REF02-PT-125</t>
+          <t>REFORMER 2</t>
         </is>
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t>PT-6027</t>
+          <t>REF02-SV-24VDC</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>--</t>
         </is>
       </c>
     </row>
@@ -2085,27 +2171,27 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>PRESSURE</t>
+          <t>POWER SUPPLY</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0.31</t>
+          <t>--</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>PT</t>
+          <t>PSU</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>24V 10A</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -2120,32 +2206,37 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>YOKOGAWA</t>
+          <t>5</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>CFU</t>
+          <t>POWER SUPPLY</t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>REF02-PT-126</t>
+          <t>CHEMEX</t>
         </is>
       </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t>PT-6028</t>
+          <t>CHE-PSU-24V 10A</t>
+        </is>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>SOLA</t>
         </is>
       </c>
     </row>
@@ -2157,27 +2248,27 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>PRESSURE</t>
+          <t>SHUTOFF VALVE</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>23</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>0.32</t>
+          <t>0.7</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>PT</t>
+          <t>XV</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>150</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -2192,32 +2283,37 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>22</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>YOKOGAWA</t>
+          <t>1</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>CFU</t>
+          <t>SHUTOFF VALVE</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>REF02-PT-127</t>
+          <t>FLARE</t>
         </is>
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t>PT-6029</t>
+          <t>FLA-XV-152</t>
+        </is>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>--</t>
         </is>
       </c>
     </row>
@@ -2229,27 +2325,27 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>PRESSURE</t>
+          <t>FLAME SENSOR</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>0.33</t>
+          <t>--</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>PT</t>
+          <t>FLAME SENSOR</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>24VDC</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -2264,32 +2360,37 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>YOKOGAWA</t>
+          <t>1</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
         <is>
+          <t>FLAME SENSOR . NO NC TYPE . ANALOG OUTPUT TYPE</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
           <t>REFORMER 2</t>
         </is>
       </c>
-      <c r="M26" t="inlineStr">
-        <is>
-          <t>REF02-PT-128</t>
-        </is>
-      </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t>PT-6030</t>
+          <t>REF02-FLAME SENSOR-24VDC</t>
+        </is>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>--</t>
         </is>
       </c>
     </row>
@@ -2301,22 +2402,22 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>PRESSURE</t>
+          <t>BALL VALVE</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>0</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>0.34</t>
+          <t>0.5''</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>PT</t>
+          <t>MECHANICAL</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2336,32 +2437,37 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>YOKOGAWA</t>
+          <t>1</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>REFORMER 2</t>
+          <t>BALL VALVE</t>
         </is>
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>REF02-PT-129</t>
+          <t>SPARE</t>
         </is>
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t>PT-6031</t>
+          <t>SPA-MECHANICAL-102</t>
+        </is>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>--</t>
         </is>
       </c>
     </row>
@@ -2373,27 +2479,27 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>PRESSURE</t>
+          <t>DI CARD</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>31</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>0.35</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>PT</t>
+          <t>IO CARD</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
@@ -2408,32 +2514,37 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>YOKOGAWA</t>
+          <t>PLC</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>REFORMER 2</t>
+          <t>AB DI CARD</t>
         </is>
       </c>
       <c r="M28" t="inlineStr">
         <is>
-          <t>REF02-PT-130</t>
+          <t>REFORMER 4</t>
         </is>
       </c>
       <c r="N28" t="inlineStr">
         <is>
-          <t>PT-6032</t>
+          <t>REF02-IO CARD--</t>
+        </is>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>5069-IB18</t>
         </is>
       </c>
     </row>
@@ -2445,32 +2556,32 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>PRESSURE</t>
+          <t>CONTROL VALVE</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>32</t>
+          <t>18</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>0.36</t>
+          <t>2''-300</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>PT</t>
+          <t>CV</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>151</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>STORE 2</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
@@ -2480,32 +2591,37 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>YOKOGAWA</t>
+          <t>1</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
         <is>
+          <t>MASONEILAN CONTROL VALVE</t>
+        </is>
+      </c>
+      <c r="M29" t="inlineStr">
+        <is>
           <t>REFORMER 2</t>
         </is>
       </c>
-      <c r="M29" t="inlineStr">
-        <is>
-          <t>REF02-PT-131</t>
-        </is>
-      </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t>PT-6033</t>
+          <t>REF02-CV-151</t>
+        </is>
+      </c>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>--</t>
         </is>
       </c>
     </row>
@@ -2517,32 +2633,32 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>PRESSURE</t>
+          <t>CONTROL VALVE</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>0.37</t>
+          <t>2''-300</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>PT</t>
+          <t>CV</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>150 PSI</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>STORE 1</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
@@ -2552,32 +2668,37 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>YOKOGAWA</t>
+          <t>-</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
         <is>
+          <t>MASONEILAN CONTROL VALVE</t>
+        </is>
+      </c>
+      <c r="M30" t="inlineStr">
+        <is>
           <t>REFORMER 2</t>
         </is>
       </c>
-      <c r="M30" t="inlineStr">
-        <is>
-          <t>REF02-PT-132</t>
-        </is>
-      </c>
       <c r="N30" t="inlineStr">
         <is>
-          <t>PT-6034</t>
+          <t>REF02-CV-150 PSI</t>
+        </is>
+      </c>
+      <c r="O30" t="inlineStr">
+        <is>
+          <t>TV-6002</t>
         </is>
       </c>
     </row>
@@ -2589,27 +2710,27 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>PRESSURE</t>
+          <t>SHUTOFF VALVE</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>34</t>
+          <t>21</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>0.38</t>
+          <t>0.5</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>PT</t>
+          <t>XV</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>150</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
@@ -2624,32 +2745,37 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>22</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>YOKOGAWA</t>
+          <t>1</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>REFORMER 2</t>
+          <t>SHUTOFF VALVE</t>
         </is>
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>REF02-PT-133</t>
+          <t>FLARE</t>
         </is>
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t>PT-6035</t>
+          <t>FLA-XV-150</t>
+        </is>
+      </c>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>--</t>
         </is>
       </c>
     </row>
@@ -2661,27 +2787,27 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>PRESSURE</t>
+          <t>SHUTOFF VALVE</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>18</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>0.39</t>
+          <t>0.5</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>PT</t>
+          <t>XV</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>150</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
@@ -2696,32 +2822,37 @@
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>22</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>YOKOGAWA</t>
+          <t>1</t>
         </is>
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>REFORMER 2</t>
+          <t>SHUTOFF VALVE</t>
         </is>
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>REF02-PT-134</t>
+          <t>FLARE</t>
         </is>
       </c>
       <c r="N32" t="inlineStr">
         <is>
-          <t>PT-6036</t>
+          <t>FLA-XV-150</t>
+        </is>
+      </c>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>--</t>
         </is>
       </c>
     </row>
@@ -2733,27 +2864,27 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>PRESSURE</t>
+          <t>SOLENOID VALVE</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>36</t>
+          <t>30</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>0.40</t>
+          <t>0.5</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>PT</t>
+          <t>SV</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>24VDC</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
@@ -2768,32 +2899,37 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>YOKOGAWA</t>
+          <t>1</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
         <is>
+          <t>SOLENOID VALVE SPARE FROM REF02</t>
+        </is>
+      </c>
+      <c r="M33" t="inlineStr">
+        <is>
           <t>REFORMER 2</t>
         </is>
       </c>
-      <c r="M33" t="inlineStr">
-        <is>
-          <t>REF02-PT-135</t>
-        </is>
-      </c>
       <c r="N33" t="inlineStr">
         <is>
-          <t>PT-6037</t>
+          <t>REF02-SV-24VDC</t>
+        </is>
+      </c>
+      <c r="O33" t="inlineStr">
+        <is>
+          <t>--</t>
         </is>
       </c>
     </row>
@@ -2805,27 +2941,27 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>PRESSURE</t>
+          <t>SHUTOFF VALVE</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>37</t>
+          <t>21</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>0.41</t>
+          <t>0.5</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>PT</t>
+          <t>XV</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>150</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
@@ -2840,32 +2976,37 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>22</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>YOKOGAWA</t>
+          <t>1</t>
         </is>
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>REFORMER 2</t>
+          <t>SHUTOFF VALVE</t>
         </is>
       </c>
       <c r="M34" t="inlineStr">
         <is>
-          <t>REF02-PT-136</t>
+          <t>FLARE</t>
         </is>
       </c>
       <c r="N34" t="inlineStr">
         <is>
-          <t>PT-6038</t>
+          <t>FLA-XV-150</t>
+        </is>
+      </c>
+      <c r="O34" t="inlineStr">
+        <is>
+          <t>--</t>
         </is>
       </c>
     </row>
@@ -2877,27 +3018,27 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>PRESSURE</t>
+          <t>DI CARD</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>38</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>0.42</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>PT</t>
+          <t>IO CARD</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
@@ -2912,32 +3053,37 @@
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>YOKOGAWA</t>
+          <t>PLC</t>
         </is>
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>REFORMER 2</t>
+          <t>AB DI CARD</t>
         </is>
       </c>
       <c r="M35" t="inlineStr">
         <is>
-          <t>REF02-PT-137</t>
+          <t>REFORMER 4</t>
         </is>
       </c>
       <c r="N35" t="inlineStr">
         <is>
-          <t>PT-6039</t>
+          <t>REF-IO CARD--</t>
+        </is>
+      </c>
+      <c r="O35" t="inlineStr">
+        <is>
+          <t>5069-IB18</t>
         </is>
       </c>
     </row>
@@ -2949,27 +3095,27 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>PRESSURE</t>
+          <t>FLAME SENSOR</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>39</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>0.43</t>
+          <t>--</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>PT</t>
+          <t>FLAME SENSOR</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>24VDC</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
@@ -2984,32 +3130,37 @@
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>YOKOGAWA</t>
+          <t>1</t>
         </is>
       </c>
       <c r="L36" t="inlineStr">
         <is>
+          <t>FLAME SENSOR . NO NC TYPE . ANALOG OUTPUT TYPE</t>
+        </is>
+      </c>
+      <c r="M36" t="inlineStr">
+        <is>
           <t>REFORMER 2</t>
         </is>
       </c>
-      <c r="M36" t="inlineStr">
-        <is>
-          <t>REF02-PT-138</t>
-        </is>
-      </c>
       <c r="N36" t="inlineStr">
         <is>
-          <t>PT-6040</t>
+          <t>REF02-FLAME SENSOR-24VDC</t>
+        </is>
+      </c>
+      <c r="O36" t="inlineStr">
+        <is>
+          <t>--</t>
         </is>
       </c>
     </row>
@@ -3021,32 +3172,32 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>PRESSURE</t>
+          <t>CONTROL VALVE</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>12</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>0.44</t>
+          <t>2''</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>PT</t>
+          <t>CV</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>150</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>STORE 1</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
@@ -3056,32 +3207,37 @@
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>YOKOGAWA</t>
+          <t>1</t>
         </is>
       </c>
       <c r="L37" t="inlineStr">
         <is>
+          <t>MASONEILAN CONTROL VALVE</t>
+        </is>
+      </c>
+      <c r="M37" t="inlineStr">
+        <is>
           <t>REFORMER 2</t>
         </is>
       </c>
-      <c r="M37" t="inlineStr">
-        <is>
-          <t>REF02-PT-139</t>
-        </is>
-      </c>
       <c r="N37" t="inlineStr">
         <is>
-          <t>PT-6041</t>
+          <t>REF02-CV-150</t>
+        </is>
+      </c>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>--</t>
         </is>
       </c>
     </row>
@@ -3093,27 +3249,27 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>PRESSURE</t>
+          <t>DI CARD</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>41</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>0.45</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>PT</t>
+          <t>IO CARD</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
@@ -3128,32 +3284,37 @@
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>YOKOGAWA</t>
+          <t>PLC</t>
         </is>
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>REFORMER 2</t>
+          <t>AB DI CARD</t>
         </is>
       </c>
       <c r="M38" t="inlineStr">
         <is>
-          <t>REF02-PT-140</t>
+          <t>REFORMER 4</t>
         </is>
       </c>
       <c r="N38" t="inlineStr">
         <is>
-          <t>PT-6042</t>
+          <t>REF-IO CARD--</t>
+        </is>
+      </c>
+      <c r="O38" t="inlineStr">
+        <is>
+          <t>5069-IB18</t>
         </is>
       </c>
     </row>
@@ -3165,27 +3326,27 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>PRESSURE</t>
+          <t>Temperature</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>42</t>
+          <t>80</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>0.46</t>
+          <t>0.5</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>PT</t>
+          <t>TT</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>600F</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
@@ -3195,37 +3356,42 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>43</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>YOKOGAWA</t>
+          <t>1</t>
         </is>
       </c>
       <c r="L39" t="inlineStr">
         <is>
+          <t>Temperature Transmitter</t>
+        </is>
+      </c>
+      <c r="M39" t="inlineStr">
+        <is>
           <t>REFORMER 2</t>
         </is>
       </c>
-      <c r="M39" t="inlineStr">
-        <is>
-          <t>REF02-PT-141</t>
-        </is>
-      </c>
       <c r="N39" t="inlineStr">
         <is>
-          <t>PT-6043</t>
+          <t>REF02-TT-600F</t>
+        </is>
+      </c>
+      <c r="O39" t="inlineStr">
+        <is>
+          <t>TT-6021</t>
         </is>
       </c>
     </row>
@@ -3237,1289 +3403,72 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>PRESSURE</t>
+          <t>Temperature</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
+          <t>210</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>0.5</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>TT</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>600F</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
           <t>43</t>
         </is>
       </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>0.47</t>
-        </is>
-      </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>PT</t>
-        </is>
-      </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="H40" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>YOKOGAWA</t>
+          <t>1</t>
         </is>
       </c>
       <c r="L40" t="inlineStr">
         <is>
+          <t>Temperature Transmitter</t>
+        </is>
+      </c>
+      <c r="M40" t="inlineStr">
+        <is>
           <t>REFORMER 2</t>
         </is>
       </c>
-      <c r="M40" t="inlineStr">
-        <is>
-          <t>REF02-PT-142</t>
-        </is>
-      </c>
       <c r="N40" t="inlineStr">
         <is>
-          <t>PT-6044</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>000040</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>PRESSURE</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>44</t>
-        </is>
-      </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>0.48</t>
-        </is>
-      </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>PT</t>
-        </is>
-      </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="H41" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I41" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="J41" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K41" t="inlineStr">
-        <is>
-          <t>YOKOGAWA</t>
-        </is>
-      </c>
-      <c r="L41" t="inlineStr">
-        <is>
-          <t>REFORMER 2</t>
-        </is>
-      </c>
-      <c r="M41" t="inlineStr">
-        <is>
-          <t>REF02-PT-143</t>
-        </is>
-      </c>
-      <c r="N41" t="inlineStr">
-        <is>
-          <t>PT-6045</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>000041</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>PRESSURE</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>45</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>0.49</t>
-        </is>
-      </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>PT</t>
-        </is>
-      </c>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="H42" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I42" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="J42" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K42" t="inlineStr">
-        <is>
-          <t>YOKOGAWA</t>
-        </is>
-      </c>
-      <c r="L42" t="inlineStr">
-        <is>
-          <t>REFORMER 2</t>
-        </is>
-      </c>
-      <c r="M42" t="inlineStr">
-        <is>
-          <t>REF02-PT-144</t>
-        </is>
-      </c>
-      <c r="N42" t="inlineStr">
-        <is>
-          <t>PT-6046</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>000042</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>PRESSURE</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>46</t>
-        </is>
-      </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>0.50</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>PT</t>
-        </is>
-      </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="H43" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I43" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="J43" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K43" t="inlineStr">
-        <is>
-          <t>YOKOGAWA</t>
-        </is>
-      </c>
-      <c r="L43" t="inlineStr">
-        <is>
-          <t>REFORMER 2</t>
-        </is>
-      </c>
-      <c r="M43" t="inlineStr">
-        <is>
-          <t>REF02-PT-145</t>
-        </is>
-      </c>
-      <c r="N43" t="inlineStr">
-        <is>
-          <t>PT-6047</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>000043</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>PRESSURE</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>0.10</t>
-        </is>
-      </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>PT</t>
-        </is>
-      </c>
-      <c r="F44" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="H44" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I44" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="J44" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K44" t="inlineStr">
-        <is>
-          <t>YOKOGAWA
-masoneilan
-rosemount</t>
-        </is>
-      </c>
-      <c r="L44" t="inlineStr">
-        <is>
-          <t>REFORMER 2</t>
-        </is>
-      </c>
-      <c r="M44" t="inlineStr">
-        <is>
-          <t>REF02-PT-105</t>
-        </is>
-      </c>
-      <c r="N44" t="inlineStr">
-        <is>
-          <t>PT-6007</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>000044</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>PRESSURE</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>0.5</t>
-        </is>
-      </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>PT</t>
-        </is>
-      </c>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="H45" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I45" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="J45" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K45" t="inlineStr">
-        <is>
-          <t>YOKOGAWA</t>
-        </is>
-      </c>
-      <c r="L45" t="inlineStr">
-        <is>
-          <t>REFORMER 2</t>
-        </is>
-      </c>
-      <c r="M45" t="inlineStr">
-        <is>
-          <t>REF02-PT-102</t>
-        </is>
-      </c>
-      <c r="N45" t="inlineStr">
-        <is>
-          <t>PT-6002</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>000045</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>pressure</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>0.5</t>
-        </is>
-      </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>PT</t>
-        </is>
-      </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>150</t>
-        </is>
-      </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="H46" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I46" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="J46" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K46" t="inlineStr">
-        <is>
-          <t>YOKOGAWA</t>
-        </is>
-      </c>
-      <c r="L46" t="inlineStr">
-        <is>
-          <t>REFORMER 2</t>
-        </is>
-      </c>
-      <c r="M46" t="inlineStr">
-        <is>
-          <t>REF02-PT-150</t>
-        </is>
-      </c>
-      <c r="N46" t="inlineStr">
-        <is>
-          <t>PT-6060</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>000046</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>PRESSURE</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>FLANGE</t>
-        </is>
-      </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>150</t>
-        </is>
-      </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="H47" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I47" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="J47" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K47" t="inlineStr">
-        <is>
-          <t>FLANGE</t>
-        </is>
-      </c>
-      <c r="L47" t="inlineStr">
-        <is>
-          <t>CRUD</t>
-        </is>
-      </c>
-      <c r="M47" t="inlineStr">
-        <is>
-          <t>CRU-FLANGE-150</t>
-        </is>
-      </c>
-      <c r="N47" t="inlineStr">
-        <is>
-          <t>PT-6067</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>000047</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>PRESSURE</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>0.9</t>
-        </is>
-      </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>PT</t>
-        </is>
-      </c>
-      <c r="F48" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="H48" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I48" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="J48" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K48" t="inlineStr">
-        <is>
-          <t>YOKOGAWA</t>
-        </is>
-      </c>
-      <c r="L48" t="inlineStr">
-        <is>
-          <t>REFORMER 6</t>
-        </is>
-      </c>
-      <c r="M48" t="inlineStr">
-        <is>
-          <t>REF-PT-100</t>
-        </is>
-      </c>
-      <c r="N48" t="inlineStr">
-        <is>
-          <t>PT-6006</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>000048</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>PRESSURE</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>0.14</t>
-        </is>
-      </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>PT</t>
-        </is>
-      </c>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="H49" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I49" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="J49" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K49" t="inlineStr">
-        <is>
-          <t>YOKOGAWA</t>
-        </is>
-      </c>
-      <c r="L49" t="inlineStr">
-        <is>
-          <t>REFORMER 11</t>
-        </is>
-      </c>
-      <c r="M49" t="inlineStr">
-        <is>
-          <t>REF-PT-100</t>
-        </is>
-      </c>
-      <c r="N49" t="inlineStr">
-        <is>
-          <t>PT-6011</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>000049</t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>pressure</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>0.5</t>
-        </is>
-      </c>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>PT</t>
-        </is>
-      </c>
-      <c r="F50" t="inlineStr">
-        <is>
-          <t>150</t>
-        </is>
-      </c>
-      <c r="G50" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="H50" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I50" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="J50" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K50" t="inlineStr">
-        <is>
-          <t>YOKOGAWA</t>
-        </is>
-      </c>
-      <c r="L50" t="inlineStr">
-        <is>
-          <t>REFORMER 2</t>
-        </is>
-      </c>
-      <c r="M50" t="inlineStr">
-        <is>
-          <t>REF02-PT-150</t>
-        </is>
-      </c>
-      <c r="N50" t="inlineStr">
-        <is>
-          <t>PT-6060</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>000050</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>PUSH FITTING</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>0.5</t>
-        </is>
-      </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>--</t>
-        </is>
-      </c>
-      <c r="F51" t="inlineStr">
-        <is>
-          <t>--</t>
-        </is>
-      </c>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="H51" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I51" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="J51" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K51" t="inlineStr">
-        <is>
-          <t>PUSH FITTING PNEUMATIC</t>
-        </is>
-      </c>
-      <c r="L51" t="inlineStr">
-        <is>
-          <t>REFORMER 2</t>
-        </is>
-      </c>
-      <c r="M51" t="inlineStr">
-        <is>
-          <t>REF02------</t>
-        </is>
-      </c>
-      <c r="N51" t="inlineStr">
-        <is>
-          <t>--</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>000051</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>PRESSURE</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>31</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>0.35</t>
-        </is>
-      </c>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>PT</t>
-        </is>
-      </c>
-      <c r="F52" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
-      <c r="G52" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="H52" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I52" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="J52" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K52" t="inlineStr">
-        <is>
-          <t>YOKOGAWA</t>
-        </is>
-      </c>
-      <c r="L52" t="inlineStr">
-        <is>
-          <t>REFORMER 32</t>
-        </is>
-      </c>
-      <c r="M52" t="inlineStr">
-        <is>
-          <t>REF-PT-100</t>
-        </is>
-      </c>
-      <c r="N52" t="inlineStr">
-        <is>
-          <t>PT-6032</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="n">
-        <v>52</v>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>PRESSURE TRANSMITTER</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>0.28</t>
-        </is>
-      </c>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>PT</t>
-        </is>
-      </c>
-      <c r="F53" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
-      <c r="G53" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="H53" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I53" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="J53" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K53" t="inlineStr">
-        <is>
-          <t>YOKOGAWA</t>
-        </is>
-      </c>
-      <c r="L53" t="inlineStr">
-        <is>
-          <t>REFORMER 2</t>
-        </is>
-      </c>
-      <c r="M53" t="inlineStr">
-        <is>
-          <t>REF02-PT-100</t>
-        </is>
-      </c>
-      <c r="N53" t="inlineStr">
-        <is>
-          <t>PT-6088</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="n">
-        <v>53</v>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>PRESSURE TRANSMITTER</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>0.5</t>
-        </is>
-      </c>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>pt</t>
-        </is>
-      </c>
-      <c r="F54" t="inlineStr">
-        <is>
-          <t>150</t>
-        </is>
-      </c>
-      <c r="G54" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="H54" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I54" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="J54" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K54" t="inlineStr">
-        <is>
-          <t>YOKOGAWA PRESSURE TRANSMITTER</t>
-        </is>
-      </c>
-      <c r="L54" t="inlineStr">
-        <is>
-          <t>REFORMER 2</t>
-        </is>
-      </c>
-      <c r="M54" t="inlineStr">
-        <is>
-          <t>REF02-PT-150</t>
-        </is>
-      </c>
-      <c r="N54" t="inlineStr">
-        <is>
-          <t>PT-6033</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>000054</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>PRESSURE TRANSMITTER</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>0.5</t>
-        </is>
-      </c>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>PT</t>
-        </is>
-      </c>
-      <c r="F55" t="inlineStr">
-        <is>
-          <t>150</t>
-        </is>
-      </c>
-      <c r="G55" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="H55" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I55" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="J55" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K55" t="inlineStr">
-        <is>
-          <t>YOKOGAWA PRESSURE TRANSMITTER</t>
-        </is>
-      </c>
-      <c r="L55" t="inlineStr">
-        <is>
-          <t>REFORMER 2</t>
-        </is>
-      </c>
-      <c r="M55" t="inlineStr">
-        <is>
-          <t>REF02-PT-150</t>
-        </is>
-      </c>
-      <c r="N55" t="inlineStr">
-        <is>
-          <t>PT-6048</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>000055</t>
-        </is>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>PRESSURE TRANSMITTER</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>0.5</t>
-        </is>
-      </c>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>PT</t>
-        </is>
-      </c>
-      <c r="F56" t="inlineStr">
-        <is>
-          <t>150</t>
-        </is>
-      </c>
-      <c r="G56" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="H56" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I56" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="J56" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K56" t="inlineStr">
-        <is>
-          <t>YOKOGAWA PRESSURE TRANSMITTER</t>
-        </is>
-      </c>
-      <c r="L56" t="inlineStr">
-        <is>
-          <t>REFORMER 2</t>
-        </is>
-      </c>
-      <c r="M56" t="inlineStr">
-        <is>
-          <t>REF02-PT-150</t>
-        </is>
-      </c>
-      <c r="N56" t="inlineStr">
-        <is>
-          <t>PT-6050</t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>000056</t>
-        </is>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>CONTROL VALVE</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>CONTROL VALVE</t>
-        </is>
-      </c>
-      <c r="F57" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G57" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="H57" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I57" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="J57" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K57" t="inlineStr">
-        <is>
-          <t>CONTROL VALVE - MASONEILAN</t>
-        </is>
-      </c>
-      <c r="L57" t="inlineStr">
-        <is>
-          <t>REFORMER 2</t>
-        </is>
-      </c>
-      <c r="M57" t="inlineStr">
-        <is>
-          <t>REF02-CONTROL VALVE--</t>
-        </is>
-      </c>
-      <c r="N57" t="inlineStr">
-        <is>
-          <t>TV-6002</t>
+          <t>REF02-TT-600F</t>
+        </is>
+      </c>
+      <c r="O40" t="inlineStr">
+        <is>
+          <t>TT-6021</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update to DB Ready
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q30"/>
+  <dimension ref="A1:Q32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -521,10 +521,8 @@
       </c>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="E2" t="n">
+        <v>4</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -604,10 +602,8 @@
         </is>
       </c>
       <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="E3" t="n">
+        <v>1</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -683,10 +679,8 @@
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="E4" t="n">
+        <v>2</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -762,10 +756,8 @@
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="E5" t="n">
+        <v>2</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -841,10 +833,8 @@
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="E6" t="n">
+        <v>2</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -924,10 +914,8 @@
         </is>
       </c>
       <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="E7" t="n">
+        <v>1</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -1007,10 +995,8 @@
         </is>
       </c>
       <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="E8" t="n">
+        <v>1</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -1094,10 +1080,8 @@
           <t>1734-IB8</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="E9" t="n">
+        <v>1</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -1177,10 +1161,8 @@
           <t>1734-OE4C</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="E10" t="n">
+        <v>1</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -1260,10 +1242,8 @@
           <t>1734-OB8</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="E11" t="n">
+        <v>1</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -1343,10 +1323,8 @@
           <t>1734-IE8C</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="E12" t="n">
+        <v>1</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -1426,10 +1404,8 @@
           <t>1734-TOP</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="E13" t="n">
+        <v>1</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
@@ -1505,10 +1481,8 @@
           <t>495905E5</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="E14" t="n">
+        <v>1</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
@@ -1588,10 +1562,8 @@
           <t>7RQ0201-1BX00</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="E15" t="n">
+        <v>3</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -1671,10 +1643,8 @@
           <t>OMRON</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="E16" t="n">
+        <v>2</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
@@ -1750,10 +1720,8 @@
         </is>
       </c>
       <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="E17" t="n">
+        <v>1</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
@@ -1833,10 +1801,8 @@
           <t>EC7823</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="E18" t="n">
+        <v>5</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
@@ -1916,10 +1882,8 @@
           <t>F06-SA6</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="E19" t="n">
+        <v>1</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
@@ -1995,10 +1959,8 @@
           <t>6006</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="E20" t="n">
+        <v>1</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -2078,10 +2040,8 @@
           <t>6026</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="E21" t="n">
+        <v>3</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
@@ -2161,10 +2121,8 @@
           <t>GGW 150 A4/2X</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="E22" t="n">
+        <v>2</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
@@ -2244,10 +2202,8 @@
           <t>LC3050</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="E23" t="n">
+        <v>2</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
@@ -2327,10 +2283,8 @@
           <t>ETCRAT00755</t>
         </is>
       </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="E24" t="n">
+        <v>1</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
@@ -2406,10 +2360,8 @@
           <t>A10</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="E25" t="n">
+        <v>1</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
@@ -2489,10 +2441,8 @@
           <t>321H2322</t>
         </is>
       </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="E26" t="n">
+        <v>1</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
@@ -2568,10 +2518,8 @@
           <t>3RU2116-1JB0</t>
         </is>
       </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="E27" t="n">
+        <v>1</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
@@ -2651,10 +2599,8 @@
           <t>3RT2016-1APO1</t>
         </is>
       </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="E28" t="n">
+        <v>1</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
@@ -2730,10 +2676,8 @@
           <t>ZA 20 100 LH 21</t>
         </is>
       </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="E29" t="n">
+        <v>2</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
@@ -2801,10 +2745,8 @@
       </c>
       <c r="C30" t="inlineStr"/>
       <c r="D30" t="inlineStr"/>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="E30" t="n">
+        <v>2</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
@@ -2858,6 +2800,164 @@
         </is>
       </c>
       <c r="Q30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>000030</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>PILOT IGNITION</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr"/>
+      <c r="D31" t="inlineStr"/>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>IGNITION</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>H-302</t>
+        </is>
+      </c>
+      <c r="N31" t="inlineStr">
+        <is>
+          <t>PILOT IGNITION</t>
+        </is>
+      </c>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>BTX</t>
+        </is>
+      </c>
+      <c r="P31" t="inlineStr">
+        <is>
+          <t>IG-ROD-PILOT</t>
+        </is>
+      </c>
+      <c r="Q31" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>000031</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>IGNITION TRANSFORMER</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>SIEMENS</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>ZA 20 100 LH 21</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>TRANSFORMER</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>220VAC</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>BOILER</t>
+        </is>
+      </c>
+      <c r="N32" t="inlineStr"/>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>BOILER</t>
+        </is>
+      </c>
+      <c r="P32" t="inlineStr">
+        <is>
+          <t>IG-XF-SIEMENS-ZA 20 100 LH 21</t>
+        </is>
+      </c>
+      <c r="Q32" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>